<commit_message>
after git issue for pressure div
</commit_message>
<xml_diff>
--- a/Adimensionnement.xlsx
+++ b/Adimensionnement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blagn771\Documents\Aquaman\Aquaman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF01B3C-5C62-4300-8C0E-680E114E2B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD85A0AC-1274-463A-B15F-81372CC9124D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CECACC56-8669-4314-B5FA-FCBDC609E522}"/>
   </bookViews>
@@ -882,7 +882,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,14 +1243,14 @@
       </c>
       <c r="B19" s="1">
         <f>F19*B29*(A4/E4)*(A4/E4)</f>
-        <v>4.0595124999999994</v>
+        <v>2.4357074999999999</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="17">
         <v>1</v>
       </c>
       <c r="F19" s="6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G19" s="6"/>
     </row>
@@ -1457,21 +1457,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100343AB94E490C1E469C434E1FE83E21E8" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4a945fd916df10b55939949b74db3e29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="30d683a2-8968-4bab-ab75-5e7ac92a4140" xmlns:ns4="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbc927056a0449b4a4b3a2dffbac1a7b" ns3:_="" ns4:_="">
     <xsd:import namespace="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
@@ -1660,32 +1645,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34829991-9D63-4183-9B9C-943F3B063F3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B68D42E-578E-4170-BB84-2395EC602713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0FF6427-00C3-42B9-A2FD-9CEA3CD59193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1702,4 +1677,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B68D42E-578E-4170-BB84-2395EC602713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34829991-9D63-4183-9B9C-943F3B063F3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Comparing sim w/ sensors
</commit_message>
<xml_diff>
--- a/Adimensionnement.xlsx
+++ b/Adimensionnement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blagn771\Documents\Aquaman\Aquaman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD85A0AC-1274-463A-B15F-81372CC9124D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030D8A19-52D4-4CCB-AE5C-8C0E82086897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CECACC56-8669-4314-B5FA-FCBDC609E522}"/>
+    <workbookView xWindow="28680" yWindow="-5205" windowWidth="16440" windowHeight="28440" xr2:uid="{CECACC56-8669-4314-B5FA-FCBDC609E522}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -882,7 +882,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,8 +1242,8 @@
         <v>4.0595124999999994</v>
       </c>
       <c r="B19" s="1">
-        <f>F19*B29*(A4/E4)*(A4/E4)</f>
-        <v>2.4357074999999999</v>
+        <f>F19*B29*(A4/E4)*(A4/E4)/2</f>
+        <v>1.21785375</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="17">
@@ -1457,6 +1457,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100343AB94E490C1E469C434E1FE83E21E8" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4a945fd916df10b55939949b74db3e29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="30d683a2-8968-4bab-ab75-5e7ac92a4140" xmlns:ns4="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbc927056a0449b4a4b3a2dffbac1a7b" ns3:_="" ns4:_="">
     <xsd:import namespace="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
@@ -1645,22 +1660,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34829991-9D63-4183-9B9C-943F3B063F3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B68D42E-578E-4170-BB84-2395EC602713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0FF6427-00C3-42B9-A2FD-9CEA3CD59193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1677,29 +1702,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B68D42E-578E-4170-BB84-2395EC602713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34829991-9D63-4183-9B9C-943F3B063F3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
loop for the tank and correction for the simu
</commit_message>
<xml_diff>
--- a/Adimensionnement.xlsx
+++ b/Adimensionnement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blagn771\Documents\Aquaman\Aquaman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030D8A19-52D4-4CCB-AE5C-8C0E82086897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAF2BF5-2A9F-47D5-ACB6-5CA9B0158399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5205" windowWidth="16440" windowHeight="28440" xr2:uid="{CECACC56-8669-4314-B5FA-FCBDC609E522}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CECACC56-8669-4314-B5FA-FCBDC609E522}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
     <t>eau de mer</t>
   </si>
   <si>
-    <t>25 deg</t>
+    <t>angle</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -565,6 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,7 +883,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +967,7 @@
       <c r="G4" s="6"/>
       <c r="I4" s="24">
         <f>I9*E4</f>
-        <v>96</v>
+        <v>7.1199999999999999E-2</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="23">
@@ -1048,6 +1049,9 @@
       <c r="G8" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="H8" s="27" t="s">
+        <v>79</v>
+      </c>
       <c r="I8" s="24" t="s">
         <v>56</v>
       </c>
@@ -1065,7 +1069,7 @@
       <c r="B9" s="13"/>
       <c r="C9" s="1">
         <f>2*G9*A9</f>
-        <v>6.6358399999999998E-2</v>
+        <v>8.21642874159451E-2</v>
       </c>
       <c r="E9" s="17">
         <v>1</v>
@@ -1075,18 +1079,19 @@
         <v>0</v>
       </c>
       <c r="G9" s="6">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="H9" t="s">
-        <v>79</v>
+        <f>H10</f>
+        <v>0.57699640039287292</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
       </c>
       <c r="I9" s="24">
-        <f>3*2^5</f>
-        <v>96</v>
+        <f>0.0712</f>
+        <v>7.1199999999999999E-2</v>
       </c>
       <c r="J9" s="25">
         <f>A9/I9</f>
-        <v>7.4166666666666662E-4</v>
+        <v>1</v>
       </c>
       <c r="K9" s="23">
         <f>B9/J9</f>
@@ -1109,6 +1114,10 @@
       </c>
       <c r="G10" s="6" t="s">
         <v>32</v>
+      </c>
+      <c r="H10">
+        <f>TAN(H9*3.14/180)</f>
+        <v>0.57699640039287292</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>57</v>
@@ -1179,7 +1188,7 @@
       <c r="C14" s="1"/>
       <c r="E14" s="17">
         <f>A14*C9/A4</f>
-        <v>0.61139199999999994</v>
+        <v>0.75701927731544916</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1457,21 +1466,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100343AB94E490C1E469C434E1FE83E21E8" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="4a945fd916df10b55939949b74db3e29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="30d683a2-8968-4bab-ab75-5e7ac92a4140" xmlns:ns4="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbc927056a0449b4a4b3a2dffbac1a7b" ns3:_="" ns4:_="">
     <xsd:import namespace="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
@@ -1660,32 +1654,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34829991-9D63-4183-9B9C-943F3B063F3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B68D42E-578E-4170-BB84-2395EC602713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0FF6427-00C3-42B9-A2FD-9CEA3CD59193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1702,4 +1686,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B68D42E-578E-4170-BB84-2395EC602713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34829991-9D63-4183-9B9C-943F3B063F3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="30d683a2-8968-4bab-ab75-5e7ac92a4140"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7b0f1024-a4c1-45bb-9adb-e11bcfb15c5a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>